<commit_message>
Rewrite to only consider exceptions
</commit_message>
<xml_diff>
--- a/fourPolar-io/src/test/resources/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/SampleImageSetByExcelFileFinder/FourCamera/TemplateFourCamera.xlsx
+++ b/fourPolar-io/src/test/resources/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/SampleImageSetByExcelFileFinder/FourCamera/TemplateFourCamera.xlsx
@@ -28,88 +28,88 @@
     <t xml:space="preserve">The path must be the remaining path after the root folder.</t>
   </si>
   <si>
-    <t xml:space="preserve">pol0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pol45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pol90</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pol135</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/FourCamera/Img1_C1_Pol0.tif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/FourCamera/Img1_C1_Pol45.tif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/FourCamera/Img1_C1_Pol90.tif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/FourCamera/Img1_C1_Pol135.tif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/FourCamera/Img2_C1_Pol0.tif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/FourCamera/Img2_C1_Pol45.tif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/FourCamera/Img2_C1_Pol90.tif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/FourCamera/Img2_C1_Pol135.tif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/FourCamera/Img3_C1_Pol0.tif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/FourCamera/Img3_C1_Pol45.tif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/FourCamera/Img3_C1_Pol90.tif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/FourCamera/Img3_C1_Pol135.tif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/FourCamera/Img4_C1_Pol0.tif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/FourCamera/Img4_C1_Pol45.tif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/FourCamera/Img4_C1_Pol90.tif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/FourCamera/Img4_C1_Pol135.tif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/FourCamera/Img5_C1_Pol0.tif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/FourCamera/Img5_C1_Pol45.tif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/FourCamera/Img5_C1_Pol90.tif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/FourCamera/Img5_C1_Pol135.tif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/FourCamera/Img6_C1_Pol0.tif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/FourCamera/Img6_C1_Pol45.tif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/FourCamera/Img6_C1_Pol90.tif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/FourCamera/Img6_C1_Pol135.tif</t>
+    <t xml:space="preserve">Pol0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pol45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pol90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pol135</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/SampleImageSetByExcelFileFinder/FourCamera/Img1_C1_Pol0.tif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/SampleImageSetByExcelFileFinder/FourCamera/Img1_C1_Pol45.tif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/SampleImageSetByExcelFileFinder/FourCamera/Img1_C1_Pol90.tif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/SampleImageSetByExcelFileFinder/FourCamera/Img1_C1_Pol135.tif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/SampleImageSetByExcelFileFinder/FourCamera/Img2_C1_Pol0.tif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/SampleImageSetByExcelFileFinder/FourCamera/Img2_C1_Pol45.tif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/SampleImageSetByExcelFileFinder/FourCamera/Img2_C1_Pol90.tif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/SampleImageSetByExcelFileFinder/FourCamera/Img2_C1_Pol135.tif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/SampleImageSetByExcelFileFinder/FourCamera/Img3_C1_Pol0.tif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/SampleImageSetByExcelFileFinder/FourCamera/Img3_C1_Pol45.tif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/SampleImageSetByExcelFileFinder/FourCamera/Img3_C1_Pol90.tif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/SampleImageSetByExcelFileFinder/FourCamera/Img3_C1_Pol135.tif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/SampleImageSetByExcelFileFinder/FourCamera/Img4_C1_Pol0.tif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/SampleImageSetByExcelFileFinder/FourCamera/Img4_C1_Pol45.tif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/SampleImageSetByExcelFileFinder/FourCamera/Img4_C1_Pol90.tif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/SampleImageSetByExcelFileFinder/FourCamera/Img4_C1_Pol135.tif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/SampleImageSetByExcelFileFinder/FourCamera/Img5_C1_Pol0.tif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/SampleImageSetByExcelFileFinder/FourCamera/Img5_C1_Pol45.tif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/SampleImageSetByExcelFileFinder/FourCamera/Img5_C1_Pol90.tif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/SampleImageSetByExcelFileFinder/FourCamera/Img5_C1_Pol135.tif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/SampleImageSetByExcelFileFinder/FourCamera/Img6_C1_Pol0.tif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/SampleImageSetByExcelFileFinder/FourCamera/Img6_C1_Pol45.tif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/SampleImageSetByExcelFileFinder/FourCamera/Img6_C1_Pol90.tif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/SampleImageSetByExcelFileFinder/FourCamera/Img6_C1_Pol135.tif</t>
   </si>
 </sst>
 </file>
@@ -217,10 +217,10 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.9"/>
   </cols>

</xml_diff>